<commit_message>
just commit the commit overthere, git user
</commit_message>
<xml_diff>
--- a/database/w2/1hs.xlsx
+++ b/database/w2/1hs.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -486,129 +486,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Fee150 SpinaSet1 pcsLevelN/ADifficulty0Materials- 25xBat Wing- 1xFour-leaf Clover- 50x Cloth- 25x Metal</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Anguish Sword[1 Handed Sword]</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Stat/EffectAmountATK %
-11
-Stability %
-10
-Physical Pierce %
-20
-ASPD
-900
-%
-stronger against Light
-10
-Dark Element
-0
-Guard Break %30</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>[NPC]Blacksmith : ZaldoSofya City: Blacksmith</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Fee150 SpinaSet1 pcsLevelN/ADifficulty0Materials- 25xBat Wing- 1xFour-leaf Clover- 50x Cloth- 25x Metal</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Anguish Sword[1 Handed Sword]</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Stat/EffectAmountATK %
-11
-Stability %
-10
-Physical Pierce %
-20
-ASPD
-900
-%
-stronger against Light
-10
-Dark Element
-0
-Guard Break %30</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>empty</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
           <t>Sell0 SpinaProcessunknown</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Accordion-fold Sword[1 Handed Sword]</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Stat/EffectAmountBase ATK
-1
-Aggro %
-30
-Attack MP Recovery
-3
-Base Stability %40</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>[NPC]Blacksmith : ZaldoSofya City: Blacksmith</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>SellUnknownProcessN/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Shortsword[1 Handed Sword]</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Stat/EffectAmountBase ATK
-10
-Base Stability %80</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Pico(Lv 1)Rakau Plains</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Sell1 SpinaProcess2 Metal</t>
         </is>
       </c>
     </row>

</xml_diff>